<commit_message>
Added: A lot of HTML and CSS
</commit_message>
<xml_diff>
--- a/DB.xlsx
+++ b/DB.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\0223livi\Desktop\da\WebbutvFinalProjectVL2021\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://jonkoping-my.sharepoint.com/personal/0223livi_jonkoping_se/Documents/Webbutveckling 2/slutprojekt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4736E61-18D0-4D9B-8EA4-A091D2DDD3BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="122" documentId="13_ncr:1_{E4736E61-18D0-4D9B-8EA4-A091D2DDD3BE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{BA8BCF8A-DB5B-4680-99E0-C0F522EADC61}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="166">
   <si>
     <t>TABEL:</t>
   </si>
@@ -373,6 +373,156 @@
   </si>
   <si>
     <t>$54.99</t>
+  </si>
+  <si>
+    <t>Desc</t>
+  </si>
+  <si>
+    <t>Large chassi with two large fans on the front and one on the back</t>
+  </si>
+  <si>
+    <t>Large chassi with three fans on the front</t>
+  </si>
+  <si>
+    <t>Dark large chassi with three medium-sized fans on the front</t>
+  </si>
+  <si>
+    <t>Nice transparent chassis with great potential for nice computers</t>
+  </si>
+  <si>
+    <t>Popular midtower chassis with nice design</t>
+  </si>
+  <si>
+    <t>Fresh midtower chassis</t>
+  </si>
+  <si>
+    <t>AMD's entry processor, good for less demanding applications</t>
+  </si>
+  <si>
+    <t>AMD's midrange processor, good cpu for the money</t>
+  </si>
+  <si>
+    <t>AMD's higher range of processors, good for editing and gaming</t>
+  </si>
+  <si>
+    <t>Intel mid range processor, good for gaming</t>
+  </si>
+  <si>
+    <t>Intel high range processor, good for editing</t>
+  </si>
+  <si>
+    <t>Intel's best processor, awesome for games and editing etc.</t>
+  </si>
+  <si>
+    <t>A standard and simple CPU fan that fixes the job</t>
+  </si>
+  <si>
+    <t>Nice fan from be quiet, which is also very quiet</t>
+  </si>
+  <si>
+    <t>Nice CPU fan for a good price</t>
+  </si>
+  <si>
+    <t>Simple but good water-cooled CPU fan</t>
+  </si>
+  <si>
+    <t>Good entrance card for games from AMD</t>
+  </si>
+  <si>
+    <t>Good graphics card for the money from AMD</t>
+  </si>
+  <si>
+    <t>AMD's top-rated graphics card that crushes all games</t>
+  </si>
+  <si>
+    <t>Nvidia's cheapest and best graphics card for the money</t>
+  </si>
+  <si>
+    <t>Nice graphics card from Nvidia, perfect for middle range computers</t>
+  </si>
+  <si>
+    <t>Awesome graphics card for those who are new to RTX</t>
+  </si>
+  <si>
+    <t>Nvidia's best 20 series graphics card</t>
+  </si>
+  <si>
+    <t>A perfect graphics card that crushes all AAA games with relief</t>
+  </si>
+  <si>
+    <t>Nvidia's best graphics card, which tremendously crushes all competitors</t>
+  </si>
+  <si>
+    <t>Nice motherboard for AMD socket processors</t>
+  </si>
+  <si>
+    <t>Nice motherboard from ASUS for Intel socket processors</t>
+  </si>
+  <si>
+    <t>Standard version of Windows, supports up to 128GB RAM</t>
+  </si>
+  <si>
+    <t>Top version of Windows, supports up to 2TB of RAM</t>
+  </si>
+  <si>
+    <t>500W power supply from EVGA</t>
+  </si>
+  <si>
+    <t>Reliable 600W power supply from EVGA</t>
+  </si>
+  <si>
+    <t>750W power supply that can handle everything from Corsair</t>
+  </si>
+  <si>
+    <t>850W power supply from Corsair, you will never need more watts</t>
+  </si>
+  <si>
+    <t>2x4 - 8GB DDR4-3000Mhz RAM from Corsair</t>
+  </si>
+  <si>
+    <t>2x8 - 16GB DDR4-3200Mhz RAM from Corsair</t>
+  </si>
+  <si>
+    <t>2x16 - 32GB DDR4-3200Mhz RAM from Corsair</t>
+  </si>
+  <si>
+    <t>4x8 - 32GB DDR4-3600Mhz RAM from Corsair</t>
+  </si>
+  <si>
+    <t>2x16 - 32GB DDR4-3600Mhz RAM from G.Skill</t>
+  </si>
+  <si>
+    <t>2x8 - 16GB DDR4-3600Mhz RAM from G.Skill</t>
+  </si>
+  <si>
+    <t>Fresh and small 240GB SSD from Kingston</t>
+  </si>
+  <si>
+    <t>Nice 1TB SSD from Samsung, perfect second hard drive for your computer</t>
+  </si>
+  <si>
+    <t>Good SSD of 500GB from Samsung</t>
+  </si>
+  <si>
+    <t>1TB M.2-NVME SSD from Samsung with insanely fast speeds, perfect for your gaming computer</t>
+  </si>
+  <si>
+    <t>A 500GB M.2-NVME SSD from Samsung that works perfectly for all computers</t>
+  </si>
+  <si>
+    <t>Mechanical hard drive from Seagate at 1TB, perfect for editing savings</t>
+  </si>
+  <si>
+    <t>A mechanical hard drive with a large space of 2TB</t>
+  </si>
+  <si>
+    <t>Good water-cooled CPU fan, even with nice rgb</t>
+  </si>
+  <si>
+    <t>An awesome CPU fan powered on water cooling with tripple fans for efficient cooling</t>
+  </si>
+  <si>
+    <t>Perfect motherboard from ASUS for Intel socket processors</t>
   </si>
 </sst>
 </file>
@@ -691,10 +841,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F60"/>
+  <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="F60" sqref="F60"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -704,9 +854,10 @@
     <col min="4" max="4" width="13.42578125" customWidth="1"/>
     <col min="5" max="5" width="9.140625" customWidth="1"/>
     <col min="6" max="6" width="13.5703125" customWidth="1"/>
+    <col min="7" max="7" width="86.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -714,7 +865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>2</v>
       </c>
@@ -727,8 +878,11 @@
       <c r="F2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>6</v>
       </c>
@@ -744,8 +898,11 @@
       <c r="F3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>9</v>
       </c>
@@ -758,8 +915,11 @@
       <c r="F4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>11</v>
       </c>
@@ -772,8 +932,11 @@
       <c r="F5">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>15</v>
       </c>
@@ -786,8 +949,11 @@
       <c r="F6">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>17</v>
       </c>
@@ -800,8 +966,11 @@
       <c r="F7">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>19</v>
       </c>
@@ -814,8 +983,11 @@
       <c r="F8">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>22</v>
       </c>
@@ -831,8 +1003,11 @@
       <c r="F10">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>25</v>
       </c>
@@ -845,8 +1020,11 @@
       <c r="F11">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>27</v>
       </c>
@@ -859,8 +1037,11 @@
       <c r="F12">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>29</v>
       </c>
@@ -873,8 +1054,11 @@
       <c r="F13">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>31</v>
       </c>
@@ -887,8 +1071,11 @@
       <c r="F14">
         <v>11</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>33</v>
       </c>
@@ -901,8 +1088,11 @@
       <c r="F15">
         <v>12</v>
       </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G15" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>35</v>
       </c>
@@ -918,8 +1108,11 @@
       <c r="F17">
         <v>13</v>
       </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G17" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>38</v>
       </c>
@@ -932,8 +1125,11 @@
       <c r="F18">
         <v>14</v>
       </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G18" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>40</v>
       </c>
@@ -946,8 +1142,11 @@
       <c r="F19">
         <v>15</v>
       </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G19" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>42</v>
       </c>
@@ -960,8 +1159,11 @@
       <c r="F20">
         <v>16</v>
       </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G20" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
         <v>44</v>
       </c>
@@ -974,8 +1176,11 @@
       <c r="F21">
         <v>17</v>
       </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G21" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>45</v>
       </c>
@@ -988,8 +1193,11 @@
       <c r="F22">
         <v>18</v>
       </c>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G22" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>47</v>
       </c>
@@ -1005,8 +1213,11 @@
       <c r="F24">
         <v>19</v>
       </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G24" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>50</v>
       </c>
@@ -1019,8 +1230,11 @@
       <c r="F25">
         <v>20</v>
       </c>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G25" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
         <v>52</v>
       </c>
@@ -1033,8 +1247,11 @@
       <c r="F26">
         <v>21</v>
       </c>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G26" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
         <v>54</v>
       </c>
@@ -1047,8 +1264,11 @@
       <c r="F27">
         <v>22</v>
       </c>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G27" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
         <v>56</v>
       </c>
@@ -1061,8 +1281,11 @@
       <c r="F28">
         <v>23</v>
       </c>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G28" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
         <v>58</v>
       </c>
@@ -1075,8 +1298,11 @@
       <c r="F29">
         <v>24</v>
       </c>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G29" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
         <v>60</v>
       </c>
@@ -1089,8 +1315,11 @@
       <c r="F30">
         <v>25</v>
       </c>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G30" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
         <v>62</v>
       </c>
@@ -1103,8 +1332,11 @@
       <c r="F31">
         <v>26</v>
       </c>
-    </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G31" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
         <v>64</v>
       </c>
@@ -1117,8 +1349,11 @@
       <c r="F32">
         <v>27</v>
       </c>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G32" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>66</v>
       </c>
@@ -1134,8 +1369,11 @@
       <c r="F34">
         <v>28</v>
       </c>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G34" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
         <v>69</v>
       </c>
@@ -1148,8 +1386,11 @@
       <c r="F35">
         <v>29</v>
       </c>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G35" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
         <v>71</v>
       </c>
@@ -1162,8 +1403,11 @@
       <c r="F36">
         <v>30</v>
       </c>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G36" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
         <v>73</v>
       </c>
@@ -1176,8 +1420,11 @@
       <c r="F37">
         <v>31</v>
       </c>
-    </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G37" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>75</v>
       </c>
@@ -1193,8 +1440,11 @@
       <c r="F39">
         <v>32</v>
       </c>
-    </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G39" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
         <v>78</v>
       </c>
@@ -1207,8 +1457,11 @@
       <c r="F40">
         <v>33</v>
       </c>
-    </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G40" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>80</v>
       </c>
@@ -1224,8 +1477,11 @@
       <c r="F42">
         <v>34</v>
       </c>
-    </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G42" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
         <v>83</v>
       </c>
@@ -1238,8 +1494,11 @@
       <c r="F43">
         <v>35</v>
       </c>
-    </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G43" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C44" t="s">
         <v>85</v>
       </c>
@@ -1252,8 +1511,11 @@
       <c r="F44">
         <v>36</v>
       </c>
-    </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G44" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C45" t="s">
         <v>87</v>
       </c>
@@ -1266,8 +1528,11 @@
       <c r="F45">
         <v>37</v>
       </c>
-    </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G45" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>89</v>
       </c>
@@ -1283,8 +1548,11 @@
       <c r="F47">
         <v>38</v>
       </c>
-    </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G47" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C48" t="s">
         <v>93</v>
       </c>
@@ -1297,8 +1565,11 @@
       <c r="F48">
         <v>39</v>
       </c>
-    </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G48" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C49" t="s">
         <v>94</v>
       </c>
@@ -1311,8 +1582,11 @@
       <c r="F49">
         <v>40</v>
       </c>
-    </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G49" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C50" t="s">
         <v>96</v>
       </c>
@@ -1325,8 +1599,11 @@
       <c r="F50">
         <v>41</v>
       </c>
-    </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G50" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C51" t="s">
         <v>98</v>
       </c>
@@ -1339,8 +1616,11 @@
       <c r="F51">
         <v>42</v>
       </c>
-    </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G51" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C52" t="s">
         <v>100</v>
       </c>
@@ -1353,8 +1633,11 @@
       <c r="F52">
         <v>43</v>
       </c>
-    </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G52" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>102</v>
       </c>
@@ -1370,8 +1653,11 @@
       <c r="F54">
         <v>44</v>
       </c>
-    </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G54" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C55" t="s">
         <v>105</v>
       </c>
@@ -1384,8 +1670,11 @@
       <c r="F55">
         <v>45</v>
       </c>
-    </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G55" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C56" t="s">
         <v>107</v>
       </c>
@@ -1398,8 +1687,11 @@
       <c r="F56">
         <v>46</v>
       </c>
-    </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G56" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C57" t="s">
         <v>109</v>
       </c>
@@ -1412,8 +1704,11 @@
       <c r="F57">
         <v>47</v>
       </c>
-    </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G57" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C58" t="s">
         <v>111</v>
       </c>
@@ -1426,8 +1721,11 @@
       <c r="F58">
         <v>48</v>
       </c>
-    </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G58" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C59" t="s">
         <v>113</v>
       </c>
@@ -1440,8 +1738,11 @@
       <c r="F59">
         <v>49</v>
       </c>
-    </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G59" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C60" t="s">
         <v>114</v>
       </c>
@@ -1453,6 +1754,9 @@
       </c>
       <c r="F60">
         <v>50</v>
+      </c>
+      <c r="G60" t="s">
+        <v>162</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added: Excel file and code
</commit_message>
<xml_diff>
--- a/DB.xlsx
+++ b/DB.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\0223livi\Desktop\projekt\WebbutvFinalProjectVL2021\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://jonkoping-my.sharepoint.com/personal/0223livi_jonkoping_se/Documents/Webbutveckling 2/slutprojekt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2F23638-2439-4C83-93A8-BA0BFE9C7617}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="79" documentId="13_ncr:1_{C2F23638-2439-4C83-93A8-BA0BFE9C7617}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{760E4C1E-C270-48DC-8644-7F790BBEF68F}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="213">
   <si>
     <t>PartpickerDB</t>
   </si>
@@ -54,12 +54,6 @@
     <t>Corsair SPEC DELTA</t>
   </si>
   <si>
-    <t>4.5 stars</t>
-  </si>
-  <si>
-    <t>5 stars</t>
-  </si>
-  <si>
     <t>Lian Li PC-011</t>
   </si>
   <si>
@@ -67,9 +61,6 @@
   </si>
   <si>
     <t>Phanteks Eclipse</t>
-  </si>
-  <si>
-    <t>4 stars</t>
   </si>
   <si>
     <t>CPU</t>
@@ -681,9 +672,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;kr&quot;_-;\-* #,##0.00\ &quot;kr&quot;_-;_-* &quot;-&quot;??\ &quot;kr&quot;_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -700,6 +691,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -726,11 +725,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1014,8 +1015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:H60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="93" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="B24" zoomScale="93" workbookViewId="0">
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1048,10 +1049,10 @@
         <v>4</v>
       </c>
       <c r="G2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="H2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1062,7 +1063,7 @@
         <v>6</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="E3" s="2">
         <v>4.5</v>
@@ -1071,10 +1072,10 @@
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
@@ -1082,7 +1083,7 @@
         <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E4" s="3">
         <v>5</v>
@@ -1091,10 +1092,10 @@
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="H4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -1102,7 +1103,7 @@
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="E5" s="3">
         <v>5</v>
@@ -1111,18 +1112,18 @@
         <v>2</v>
       </c>
       <c r="G5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="H5" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="E6" s="3">
         <v>5</v>
@@ -1131,18 +1132,18 @@
         <v>3</v>
       </c>
       <c r="G6" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="H6" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E7" s="3">
         <v>4</v>
@@ -1151,18 +1152,18 @@
         <v>4</v>
       </c>
       <c r="G7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="H7" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E8" s="2">
         <v>4.5</v>
@@ -1171,21 +1172,21 @@
         <v>5</v>
       </c>
       <c r="G8" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="H8" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D10" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="E10" s="3">
         <v>4</v>
@@ -1194,18 +1195,18 @@
         <v>6</v>
       </c>
       <c r="G10" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="H10" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E11" s="3">
         <v>5</v>
@@ -1214,18 +1215,18 @@
         <v>7</v>
       </c>
       <c r="G11" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H11" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D12" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E12" s="3">
         <v>5</v>
@@ -1234,18 +1235,18 @@
         <v>8</v>
       </c>
       <c r="G12" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H12" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D13" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E13" s="3">
         <v>5</v>
@@ -1254,18 +1255,18 @@
         <v>9</v>
       </c>
       <c r="G13" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H13" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D14" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E14" s="3">
         <v>5</v>
@@ -1274,18 +1275,18 @@
         <v>10</v>
       </c>
       <c r="G14" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="H14" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D15" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="E15" s="3">
         <v>5</v>
@@ -1294,795 +1295,808 @@
         <v>11</v>
       </c>
       <c r="G15" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C17" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D17" t="s">
-        <v>180</v>
-      </c>
-      <c r="E17" t="s">
-        <v>14</v>
+        <v>177</v>
+      </c>
+      <c r="E17" s="3">
+        <v>4</v>
       </c>
       <c r="F17">
         <v>12</v>
       </c>
       <c r="G17" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H17" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D18" t="s">
-        <v>181</v>
-      </c>
-      <c r="E18" t="s">
-        <v>10</v>
+        <v>178</v>
+      </c>
+      <c r="E18" s="3">
+        <v>5</v>
       </c>
       <c r="F18">
         <v>13</v>
       </c>
       <c r="G18" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="H18" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D19" t="s">
-        <v>182</v>
-      </c>
-      <c r="E19" t="s">
-        <v>14</v>
+        <v>179</v>
+      </c>
+      <c r="E19" s="3">
+        <v>4</v>
       </c>
       <c r="F19">
         <v>14</v>
       </c>
       <c r="G19" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="H19" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D20" t="s">
-        <v>183</v>
-      </c>
-      <c r="E20" t="s">
-        <v>10</v>
+        <v>180</v>
+      </c>
+      <c r="E20" s="3">
+        <v>5</v>
       </c>
       <c r="F20">
         <v>15</v>
       </c>
       <c r="G20" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="H20" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D21" t="s">
-        <v>176</v>
-      </c>
-      <c r="E21" t="s">
-        <v>10</v>
+        <v>173</v>
+      </c>
+      <c r="E21" s="3">
+        <v>5</v>
       </c>
       <c r="F21">
         <v>16</v>
       </c>
       <c r="G21" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="H21" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D22" t="s">
-        <v>184</v>
-      </c>
-      <c r="E22" t="s">
-        <v>9</v>
+        <v>181</v>
+      </c>
+      <c r="E22" s="2">
+        <v>4.5</v>
       </c>
       <c r="F22">
         <v>17</v>
       </c>
       <c r="G22" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H22" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C24" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D24" t="s">
-        <v>185</v>
-      </c>
-      <c r="E24" t="s">
-        <v>14</v>
+        <v>182</v>
+      </c>
+      <c r="E24" s="3">
+        <v>4</v>
       </c>
       <c r="F24">
         <v>18</v>
       </c>
       <c r="G24" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H24" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D25" t="s">
-        <v>186</v>
-      </c>
-      <c r="E25" t="s">
-        <v>10</v>
+        <v>183</v>
+      </c>
+      <c r="E25" s="3">
+        <v>5</v>
       </c>
       <c r="F25">
         <v>19</v>
       </c>
       <c r="G25" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="H25" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D26" t="s">
-        <v>187</v>
-      </c>
-      <c r="E26" t="s">
-        <v>10</v>
+        <v>184</v>
+      </c>
+      <c r="E26" s="3">
+        <v>5</v>
       </c>
       <c r="F26">
         <v>20</v>
       </c>
       <c r="G26" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="H26" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D27" t="s">
-        <v>188</v>
-      </c>
-      <c r="E27" t="s">
-        <v>9</v>
+        <v>185</v>
+      </c>
+      <c r="E27" s="2">
+        <v>4.5</v>
       </c>
       <c r="F27">
         <v>21</v>
       </c>
       <c r="G27" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="H27" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D28" t="s">
-        <v>189</v>
-      </c>
-      <c r="E28" t="s">
-        <v>9</v>
+        <v>186</v>
+      </c>
+      <c r="E28" s="2">
+        <v>4.5</v>
       </c>
       <c r="F28">
         <v>22</v>
       </c>
       <c r="G28" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="H28" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D29" t="s">
-        <v>190</v>
-      </c>
-      <c r="E29" t="s">
-        <v>9</v>
+        <v>187</v>
+      </c>
+      <c r="E29" s="2">
+        <v>4.5</v>
       </c>
       <c r="F29">
         <v>23</v>
       </c>
       <c r="G29" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="H29" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D30" t="s">
-        <v>191</v>
-      </c>
-      <c r="E30" t="s">
-        <v>14</v>
+        <v>188</v>
+      </c>
+      <c r="E30" s="3">
+        <v>4</v>
       </c>
       <c r="F30">
         <v>24</v>
       </c>
       <c r="G30" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="H30" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D31" t="s">
-        <v>192</v>
-      </c>
-      <c r="E31" t="s">
-        <v>10</v>
+        <v>189</v>
+      </c>
+      <c r="E31" s="3">
+        <v>5</v>
       </c>
       <c r="F31">
         <v>25</v>
       </c>
       <c r="G31" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="H31" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D32" t="s">
-        <v>193</v>
-      </c>
-      <c r="E32" t="s">
-        <v>10</v>
+        <v>190</v>
+      </c>
+      <c r="E32" s="5">
+        <v>5</v>
       </c>
       <c r="F32">
         <v>26</v>
       </c>
       <c r="G32" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="H32" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C34" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D34" t="s">
-        <v>194</v>
-      </c>
-      <c r="E34" t="s">
-        <v>9</v>
+        <v>191</v>
+      </c>
+      <c r="E34" s="2">
+        <v>4.5</v>
       </c>
       <c r="F34">
         <v>27</v>
       </c>
       <c r="G34" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="H34" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D35" t="s">
-        <v>195</v>
-      </c>
-      <c r="E35" t="s">
-        <v>10</v>
+        <v>192</v>
+      </c>
+      <c r="E35" s="2">
+        <v>5</v>
       </c>
       <c r="F35">
         <v>28</v>
       </c>
       <c r="G35" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="H35" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D36" t="s">
-        <v>196</v>
-      </c>
-      <c r="E36" t="s">
-        <v>9</v>
+        <v>193</v>
+      </c>
+      <c r="E36" s="2">
+        <v>4.5</v>
       </c>
       <c r="F36">
         <v>29</v>
       </c>
       <c r="G36" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H36" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D37" t="s">
-        <v>197</v>
-      </c>
-      <c r="E37" t="s">
-        <v>9</v>
+        <v>194</v>
+      </c>
+      <c r="E37" s="2">
+        <v>4.5</v>
       </c>
       <c r="F37">
         <v>30</v>
       </c>
       <c r="G37" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="H37" t="s">
-        <v>148</v>
-      </c>
+        <v>145</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E38" s="4"/>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C39" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D39" t="s">
-        <v>198</v>
-      </c>
-      <c r="E39" t="s">
-        <v>9</v>
+        <v>195</v>
+      </c>
+      <c r="E39" s="2">
+        <v>4.5</v>
       </c>
       <c r="F39">
         <v>31</v>
       </c>
       <c r="G39" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="H39" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D40" t="s">
-        <v>199</v>
-      </c>
-      <c r="E40" t="s">
-        <v>10</v>
+        <v>196</v>
+      </c>
+      <c r="E40" s="3">
+        <v>5</v>
       </c>
       <c r="F40">
         <v>32</v>
       </c>
       <c r="G40" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="H40" t="s">
-        <v>150</v>
-      </c>
+        <v>147</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E41" s="3"/>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C42" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D42" t="s">
-        <v>200</v>
-      </c>
-      <c r="E42" t="s">
-        <v>14</v>
+        <v>197</v>
+      </c>
+      <c r="E42" s="3">
+        <v>4</v>
       </c>
       <c r="F42">
         <v>33</v>
       </c>
       <c r="G42" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="H42" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D43" t="s">
-        <v>201</v>
-      </c>
-      <c r="E43" t="s">
-        <v>9</v>
+        <v>198</v>
+      </c>
+      <c r="E43" s="2">
+        <v>4.5</v>
       </c>
       <c r="F43">
         <v>34</v>
       </c>
       <c r="G43" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="H43" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C44" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D44" t="s">
-        <v>202</v>
-      </c>
-      <c r="E44" t="s">
-        <v>10</v>
+        <v>199</v>
+      </c>
+      <c r="E44" s="3">
+        <v>5</v>
       </c>
       <c r="F44">
         <v>35</v>
       </c>
       <c r="G44" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H44" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C45" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D45" t="s">
-        <v>203</v>
-      </c>
-      <c r="E45" t="s">
-        <v>10</v>
+        <v>200</v>
+      </c>
+      <c r="E45" s="3">
+        <v>5</v>
       </c>
       <c r="F45">
         <v>36</v>
       </c>
       <c r="G45" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H45" t="s">
-        <v>154</v>
-      </c>
+        <v>151</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E46" s="4"/>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C47" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D47" t="s">
-        <v>204</v>
-      </c>
-      <c r="E47" t="s">
-        <v>9</v>
+        <v>201</v>
+      </c>
+      <c r="E47" s="2">
+        <v>4.5</v>
       </c>
       <c r="F47">
         <v>37</v>
       </c>
       <c r="G47" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H47" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C48" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D48" t="s">
-        <v>205</v>
-      </c>
-      <c r="E48" t="s">
-        <v>9</v>
+        <v>202</v>
+      </c>
+      <c r="E48" s="2">
+        <v>4.5</v>
       </c>
       <c r="F48">
         <v>38</v>
       </c>
       <c r="G48" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="H48" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C49" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D49" t="s">
-        <v>206</v>
-      </c>
-      <c r="E49" t="s">
-        <v>10</v>
+        <v>203</v>
+      </c>
+      <c r="E49" s="3">
+        <v>5</v>
       </c>
       <c r="F49">
         <v>39</v>
       </c>
       <c r="G49" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H49" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C50" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D50" t="s">
-        <v>207</v>
-      </c>
-      <c r="E50" t="s">
-        <v>10</v>
+        <v>204</v>
+      </c>
+      <c r="E50" s="3">
+        <v>5</v>
       </c>
       <c r="F50">
         <v>40</v>
       </c>
       <c r="G50" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="H50" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C51" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D51" t="s">
-        <v>208</v>
-      </c>
-      <c r="E51" t="s">
-        <v>9</v>
+        <v>205</v>
+      </c>
+      <c r="E51" s="2">
+        <v>4.5</v>
       </c>
       <c r="F51">
         <v>41</v>
       </c>
       <c r="G51" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="H51" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C52" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D52" t="s">
-        <v>209</v>
-      </c>
-      <c r="E52" t="s">
-        <v>10</v>
+        <v>206</v>
+      </c>
+      <c r="E52" s="3">
+        <v>5</v>
       </c>
       <c r="F52">
         <v>42</v>
       </c>
       <c r="G52" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="H52" t="s">
-        <v>160</v>
-      </c>
+        <v>157</v>
+      </c>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E53" s="4"/>
     </row>
     <row r="54" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C54" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D54" t="s">
-        <v>210</v>
-      </c>
-      <c r="E54" t="s">
-        <v>9</v>
+        <v>207</v>
+      </c>
+      <c r="E54" s="2">
+        <v>4.5</v>
       </c>
       <c r="F54">
         <v>43</v>
       </c>
       <c r="G54" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="H54" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="55" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C55" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D55" t="s">
-        <v>211</v>
-      </c>
-      <c r="E55" t="s">
-        <v>9</v>
+        <v>208</v>
+      </c>
+      <c r="E55" s="2">
+        <v>4.5</v>
       </c>
       <c r="F55">
         <v>44</v>
       </c>
       <c r="G55" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="H55" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C56" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D56" t="s">
-        <v>212</v>
-      </c>
-      <c r="E56" t="s">
-        <v>14</v>
+        <v>209</v>
+      </c>
+      <c r="E56" s="3">
+        <v>4</v>
       </c>
       <c r="F56">
         <v>45</v>
       </c>
       <c r="G56" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H56" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="57" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C57" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D57" t="s">
-        <v>213</v>
-      </c>
-      <c r="E57" t="s">
-        <v>10</v>
+        <v>210</v>
+      </c>
+      <c r="E57" s="3">
+        <v>5</v>
       </c>
       <c r="F57">
         <v>46</v>
       </c>
       <c r="G57" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="H57" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="58" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C58" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D58" t="s">
-        <v>214</v>
-      </c>
-      <c r="E58" t="s">
-        <v>10</v>
+        <v>211</v>
+      </c>
+      <c r="E58" s="3">
+        <v>5</v>
       </c>
       <c r="F58">
         <v>47</v>
       </c>
       <c r="G58" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="H58" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="59" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C59" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D59" t="s">
-        <v>200</v>
-      </c>
-      <c r="E59" t="s">
-        <v>10</v>
+        <v>197</v>
+      </c>
+      <c r="E59" s="3">
+        <v>5</v>
       </c>
       <c r="F59">
         <v>48</v>
       </c>
       <c r="G59" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="H59" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="60" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C60" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D60" t="s">
-        <v>215</v>
-      </c>
-      <c r="E60" t="s">
-        <v>14</v>
+        <v>212</v>
+      </c>
+      <c r="E60" s="3">
+        <v>4</v>
       </c>
       <c r="F60">
         <v>49</v>
       </c>
       <c r="G60" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="H60" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>